<commit_message>
Update Notes and Writeoff
</commit_message>
<xml_diff>
--- a/Close.xlsx
+++ b/Close.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Innovativedell\git\repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096D9C68-EB46-490E-8013-532772EE3C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840E2C07-4986-4CE2-9E6C-4BA050204FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4668" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -358,8 +358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7647"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="B197" sqref="B197"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -378,7 +378,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>117018448</v>
+        <v>116585314</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>